<commit_message>
fix error tahap 3
</commit_message>
<xml_diff>
--- a/StemmingTala.xlsx
+++ b/StemmingTala.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>terkadang</t>
+          <t>kadang</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>kedip</t>
+          <t>dip</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>kedip</t>
+          <t>dip</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>menerang</t>
+          <t>erang</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>kertas</t>
+          <t>rtas</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>dipajang</t>
+          <t>pajang</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>mencolok</t>
+          <t>colok</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>memandang</t>
+          <t>pandang</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>menarik</t>
+          <t>arik</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ditemu</t>
+          <t>temu</t>
         </is>
       </c>
     </row>
@@ -986,7 +986,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>nyelidi</t>
+          <t>nyelid</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>memutus</t>
+          <t>putus</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>membentuk</t>
+          <t>bentuk</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>diputus</t>
+          <t>putus</t>
         </is>
       </c>
     </row>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>menambah</t>
+          <t>ambah</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>terletak</t>
+          <t>letak</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>menit</t>
+          <t>it</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>kereta</t>
+          <t>reta</t>
         </is>
       </c>
     </row>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>menjadi</t>
+          <t>jad</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>terkenal</t>
+          <t>kenal</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>belanja</t>
+          <t>anja</t>
         </is>
       </c>
     </row>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ditinggal</t>
+          <t>tinggal</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>dibanding</t>
+          <t>banding</t>
         </is>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>memilik</t>
+          <t>pilik</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>lari</t>
+          <t>lar</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>keliar</t>
+          <t>liar</t>
         </is>
       </c>
     </row>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>kejahat</t>
+          <t>jahat</t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>dikenal</t>
+          <t>kenal</t>
         </is>
       </c>
     </row>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>kekeras</t>
+          <t>keras</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>merkosa</t>
+          <t>rkosa</t>
         </is>
       </c>
     </row>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>menculik</t>
+          <t>culik</t>
         </is>
       </c>
     </row>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>membunuh</t>
+          <t>bunuh</t>
         </is>
       </c>
     </row>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>diliput</t>
+          <t>liput</t>
         </is>
       </c>
     </row>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>mencekam</t>
+          <t>cekam</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix aturan awalan1 dan awalan2
</commit_message>
<xml_diff>
--- a/StemmingTala.xlsx
+++ b/StemmingTala.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>nyelidik</t>
+          <t>selidik</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>mbunuh</t>
+          <t>bunuh</t>
         </is>
       </c>
     </row>
@@ -986,7 +986,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>nyelid</t>
+          <t>selid</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>nduduk</t>
+          <t>duduk</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>mbakar</t>
+          <t>bakar</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>rkosa</t>
+          <t>perkosa</t>
         </is>
       </c>
     </row>

</xml_diff>